<commit_message>
fix melting data exel
</commit_message>
<xml_diff>
--- a/melting data.xlsx
+++ b/melting data.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewbarr/Downloads/Python_for_Data_Analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewbarr/Python-For-Data-Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFBBFEF0-6034-A649-8F54-398610768E8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADFD927A-1806-6840-B980-71D05179296B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1880" yWindow="2460" windowWidth="25140" windowHeight="11680" xr2:uid="{BAAF6D3E-B9EA-7443-A6A7-D7063A289D46}"/>
+    <workbookView xWindow="-940" yWindow="460" windowWidth="27060" windowHeight="16140" xr2:uid="{BAAF6D3E-B9EA-7443-A6A7-D7063A289D46}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$J$3:$M$12</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -604,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFA03117-891B-DE48-B5DB-8AD4F7B217E1}">
   <dimension ref="B2:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:F9"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -715,7 +718,7 @@
         <v>5</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M5" s="6" t="s">
         <v>8</v>
@@ -744,7 +747,7 @@
         <v>5</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M6" s="6" t="s">
         <v>9</v>
@@ -758,7 +761,7 @@
         <v>5</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M7" s="6" t="s">
         <v>10</v>
@@ -800,7 +803,7 @@
         <v>5</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M9" s="6" t="s">
         <v>12</v>
@@ -814,7 +817,7 @@
         <v>6</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M10" s="6" t="s">
         <v>11</v>
@@ -828,7 +831,7 @@
         <v>6</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M11" s="6" t="s">
         <v>9</v>
@@ -841,7 +844,7 @@
       <c r="K12" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="L12" s="8" t="s">
+      <c r="L12" s="5" t="s">
         <v>3</v>
       </c>
       <c r="M12" s="9" t="s">

</xml_diff>